<commit_message>
- add button event listeners
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/form_leave.xlsx
+++ b/src/main/webapp/WEB-INF/book/form_leave.xlsx
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +87,11 @@
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="72"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="4">
@@ -159,6 +164,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -171,9 +179,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -187,6 +192,82 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1498600</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="submit" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica"/>
+                  <a:ea typeface="Helvetica"/>
+                  <a:cs typeface="Helvetica"/>
+                </a:rPr>
+                <a:t>Submit</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,11 +532,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,13 +549,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="31" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -485,11 +566,11 @@
       </c>
       <c r="F3" s="3">
         <f ca="1">TODAY()</f>
-        <v>43356</v>
+        <v>43361</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -497,42 +578,42 @@
       </c>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>43356</v>
-      </c>
-      <c r="E4" s="9" t="s">
+        <v>43361</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="11">
         <f ca="1">IF(NETWORKDAYS(D4,D5) &lt; 0, 0, NETWORKDAYS(D4,D5))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="2:6" ht="72" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" ht="24" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -544,5 +625,37 @@
     <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId3" name="submit">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>1498600</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+          <mc:Fallback/>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add logout button and its listener
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/form_leave.xlsx
+++ b/src/main/webapp/WEB-INF/book/form_leave.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33580" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Leave" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,7 +90,17 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="72"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
@@ -198,6 +208,14 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -237,8 +255,8 @@
             <a:noFill/>
             <a:ln w="9525">
               <a:miter lim="800000"/>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:headEnd/>
+              <a:tailEnd/>
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
@@ -258,6 +276,140 @@
                   <a:cs typeface="Helvetica"/>
                 </a:rPr>
                 <a:t>Submit</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>876300</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>952500</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="approve" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="00B050"/>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica"/>
+                  <a:ea typeface="Helvetica"/>
+                  <a:cs typeface="Helvetica"/>
+                </a:rPr>
+                <a:t>Approve</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>774700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="reject" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica"/>
+                  <a:ea typeface="Helvetica"/>
+                  <a:cs typeface="Helvetica"/>
+                </a:rPr>
+                <a:t>Reject</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -533,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:F6"/>
@@ -566,7 +718,7 @@
       </c>
       <c r="F3" s="3">
         <f ca="1">TODAY()</f>
-        <v>43361</v>
+        <v>43363</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="24" x14ac:dyDescent="0.2">
@@ -578,7 +730,7 @@
       </c>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>43361</v>
+        <v>43363</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>4</v>
@@ -615,6 +767,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
+    <row r="10" spans="2:6" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C7:F7"/>
@@ -653,6 +806,52 @@
           </mc:Choice>
           <mc:Fallback/>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId4" name="approve">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>876300</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>952500</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+          <mc:Fallback/>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId5" name="reject">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>774700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+          <mc:Fallback/>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
     <mc:Fallback/>

</xml_diff>

<commit_message>
- save and load owner - approve a submission
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/form_leave.xlsx
+++ b/src/main/webapp/WEB-INF/book/form_leave.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>APPLICATION FOR LEAVE</t>
   </si>
@@ -61,6 +61,9 @@
   <si>
     <t>Applicant</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Employee</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:F6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,7 +721,7 @@
       </c>
       <c r="F3" s="3">
         <f ca="1">TODAY()</f>
-        <v>43363</v>
+        <v>43364</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="24" x14ac:dyDescent="0.2">
@@ -730,7 +733,7 @@
       </c>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>43363</v>
+        <v>43364</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>4</v>
@@ -762,7 +765,9 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>

</xml_diff>

<commit_message>
* apply Lauren's new form template * remove unused template
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/form_leave.xlsx
+++ b/src/main/webapp/WEB-INF/book/form_leave.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Leave" sheetId="1" r:id="rId1"/>
@@ -29,19 +29,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>APPLICATION FOR LEAVE</t>
-  </si>
-  <si>
     <t>Period of 
 Leave</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>From</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>To</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -61,6 +50,15 @@
   </si>
   <si>
     <t>Employee</t>
+  </si>
+  <si>
+    <t>Application For Leave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To </t>
   </si>
 </sst>
 </file>
@@ -89,27 +87,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color theme="2" tint="-0.249977111117893"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Tahoma"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +132,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -153,30 +157,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color rgb="FF00B2B3"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </left>
       <right style="thin">
         <color theme="0"/>
@@ -189,38 +204,29 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF00B2B3"/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="0"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FF00B2B3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF00B2B3"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF00B2B3"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -230,7 +236,42 @@
       </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
       <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
         <color theme="0"/>
       </bottom>
       <diagonal/>
@@ -238,107 +279,14 @@
     <border>
       <left/>
       <right style="medium">
-        <color rgb="FF00B2B3"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF00B2B3"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF00B2B3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF00B2B3"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF00B2B3"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </right>
       <top style="medium">
-        <color rgb="FF00B2B3"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF00B2B3"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF00B2B3"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF00B2B3"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF00B2B3"/>
-      </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF00B2B3"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -346,29 +294,83 @@
         <color theme="0"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
       <bottom style="medium">
-        <color theme="0"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB9E7DD"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color theme="0"/>
       </top>
       <bottom/>
@@ -379,73 +381,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -456,8 +464,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFB9E7DD"/>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FF00B2B3"/>
-      <color rgb="FFB9E7DD"/>
     </mruColors>
   </colors>
   <extLst>
@@ -490,16 +499,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>5</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>50800</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>1498600</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -557,16 +566,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>1485900</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>50800</xdr:rowOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -624,16 +633,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1168400</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1130300</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>1244600</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -691,15 +700,15 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1168400</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1130300</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>1244600</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1020,107 +1029,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="2:12" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="2:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5">
+        <f ca="1">TODAY()</f>
+        <v>43378</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7">
+        <f ca="1">TODAY()</f>
+        <v>43378</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="2:12" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10">
+        <f ca="1">IF(NETWORKDAYS(E4,E5) &lt; 0, 0, NETWORKDAYS(E4,E5))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="2:12" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="2:12" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11">
-        <f ca="1">TODAY()</f>
-        <v>43375</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="8">
-        <f ca="1">TODAY()</f>
-        <v>43375</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="5">
-        <f ca="1">IF(NETWORKDAYS(D3,D4) &lt; 0, 0, NETWORKDAYS(D3,D4))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="79" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="D7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="9" spans="2:6" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="1"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="D3" unlockedFormula="1"/>
+    <ignoredError sqref="E4" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1133,16 +1306,16 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>12700</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>50800</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>1498600</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1156,16 +1329,16 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>1485900</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>50800</xdr:rowOff>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1179,16 +1352,16 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>1168400</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>1130300</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>1244600</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1202,15 +1375,15 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>1168400</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>1130300</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>1244600</xdr:colOff>
-                    <xdr:row>8</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>